<commit_message>
adding a gitignore file
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigBO_2020.xlsx
+++ b/ConfigFiles/ConfigBO_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VLIR_\Documents\git\hydro_units_bolivia\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4603FDA4-B01F-42FA-8FC0-1381AECE41CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BC350B-CB05-4C22-80CD-0B4A6CD46009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="182">
   <si>
     <t>Default value</t>
   </si>
@@ -552,19 +552,25 @@
     <t>Bolivia 2020 case study configuration file research purposes. Four zones (CE, NO, OR, SU) are simulated. The simulated period is 1 year</t>
   </si>
   <si>
+    <t>HydroData/ReservoirLevel/##/2020.csv</t>
+  </si>
+  <si>
+    <t>PowerPlants/##/2020.csv</t>
+  </si>
+  <si>
+    <t>AvailabilityFactors/##/2020.csv</t>
+  </si>
+  <si>
+    <t>HydroData/ScaledInflows/##/2020.csv</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
     <t>Simulations/bolivia_base_2020</t>
   </si>
   <si>
-    <t>HydroData/ReservoirLevel/##/2020.csv</t>
-  </si>
-  <si>
-    <t>PowerPlants/##/2020.csv</t>
-  </si>
-  <si>
-    <t>AvailabilityFactors/##/2020.csv</t>
-  </si>
-  <si>
-    <t>HydroData/ScaledInflows/##/2020.csv</t>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -1268,8 +1274,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q162" sqref="Q162"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1433,33 +1439,42 @@
         <v>60</v>
       </c>
       <c r="B16" s="29"/>
-    </row>
-    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B17" s="30"/>
-    </row>
-    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B18" s="28"/>
-    </row>
-    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C18" s="13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:3" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:3" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:8" s="38" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35" t="s">
         <v>130</v>
@@ -1480,7 +1495,7 @@
         <v>10</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -1589,7 +1604,7 @@
         <v>12</v>
       </c>
       <c r="C58" s="17">
-        <v>44196</v>
+        <v>43861</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>46</v>
@@ -1752,7 +1767,7 @@
         <v>34</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>113</v>
@@ -1905,7 +1920,7 @@
         <v>10</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>63</v>
@@ -1922,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D129" s="18" t="s">
         <v>63</v>
@@ -1989,7 +2004,7 @@
         <v>10</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D133" s="18" t="s">
         <v>63</v>
@@ -2006,7 +2021,7 @@
         <v>10</v>
       </c>
       <c r="C134" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D134" s="18" t="s">
         <v>63</v>

</xml_diff>